<commit_message>
[Added multiple document print in one workbook] [And forces user to print iwthout editing]
</commit_message>
<xml_diff>
--- a/AltasoftDaily.UserInterface.WindowsForms/new-order.xlsx
+++ b/AltasoftDaily.UserInterface.WindowsForms/new-order.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BurnOutDev\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Uploaded from Samsung Laptop\Desktop\AltasoftDaily - Copy (2)\AltasoftDaily.UserInterface.WindowsForms\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -545,7 +545,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -563,7 +563,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
@@ -593,21 +592,93 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -619,78 +690,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1114,31 +1113,31 @@
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" style="30" customWidth="1"/>
-    <col min="2" max="2" width="19" style="30" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" style="30" customWidth="1"/>
-    <col min="4" max="4" width="14" style="30" customWidth="1"/>
-    <col min="5" max="5" width="1.85546875" style="30" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" style="30" customWidth="1"/>
-    <col min="7" max="7" width="24" style="30" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="30" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" style="29" customWidth="1"/>
+    <col min="2" max="2" width="19" style="29" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="29" customWidth="1"/>
+    <col min="4" max="4" width="14" style="29" customWidth="1"/>
+    <col min="5" max="5" width="1.85546875" style="29" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" style="29" customWidth="1"/>
+    <col min="7" max="7" width="24" style="29" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="29" customWidth="1"/>
     <col min="9" max="11" width="9.140625" style="1" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1147,8 +1146,8 @@
         <v>1</v>
       </c>
       <c r="B3" s="5"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="63"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="35"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
@@ -1161,19 +1160,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="59"/>
-    </row>
-    <row r="6" spans="1:7" s="30" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C5" s="30"/>
+      <c r="D5" s="31"/>
+    </row>
+    <row r="6" spans="1:7" s="29" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="13"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="61"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="33"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" s="30" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" s="29" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
@@ -1181,177 +1180,177 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:7" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+    <row r="8" spans="1:7" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="5"/>
-      <c r="C8" s="62"/>
-      <c r="D8" s="63"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="35"/>
       <c r="E8" s="6"/>
-      <c r="F8" s="54" t="s">
+      <c r="F8" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="G8" s="50"/>
-    </row>
-    <row r="9" spans="1:7" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G8" s="48"/>
+    </row>
+    <row r="9" spans="1:7" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="17"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="16"/>
       <c r="E9" s="6"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="35"/>
-    </row>
-    <row r="10" spans="1:7" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F9" s="51"/>
+      <c r="G9" s="52"/>
+    </row>
+    <row r="10" spans="1:7" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="59"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="31"/>
       <c r="E10" s="6"/>
-      <c r="F10" s="32" t="s">
+      <c r="F10" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="G10" s="52" t="s">
+      <c r="G10" s="54" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="30" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" s="29" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="13"/>
-      <c r="C11" s="60"/>
-      <c r="D11" s="61"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="33"/>
       <c r="E11" s="6"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="53"/>
-    </row>
-    <row r="12" spans="1:7" s="30" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F11" s="51"/>
+      <c r="G11" s="55"/>
+    </row>
+    <row r="12" spans="1:7" s="29" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="14"/>
       <c r="B12" s="14"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
       <c r="E12" s="6"/>
-      <c r="F12" s="32" t="s">
+      <c r="F12" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="G12" s="34"/>
-    </row>
-    <row r="13" spans="1:7" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
+      <c r="G12" s="58"/>
+    </row>
+    <row r="13" spans="1:7" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="22"/>
-      <c r="C13" s="46"/>
-      <c r="D13" s="47"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="39"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="35"/>
-    </row>
-    <row r="14" spans="1:7" s="30" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="23"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="48"/>
-      <c r="D14" s="49"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="52"/>
+    </row>
+    <row r="14" spans="1:7" s="29" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="22"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="41"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="19"/>
-    </row>
-    <row r="15" spans="1:7" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F14" s="17"/>
+      <c r="G14" s="18"/>
+    </row>
+    <row r="15" spans="1:7" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E15" s="6"/>
-      <c r="F15" s="36" t="s">
+      <c r="F15" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="G15" s="37"/>
-    </row>
-    <row r="16" spans="1:7" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="55" t="s">
+      <c r="G15" s="60"/>
+    </row>
+    <row r="16" spans="1:7" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="55"/>
-      <c r="C16" s="55"/>
-      <c r="D16" s="55"/>
+      <c r="B16" s="56"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="56"/>
       <c r="E16" s="6"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="39"/>
-    </row>
-    <row r="17" spans="1:7" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="55"/>
-      <c r="B17" s="55"/>
-      <c r="C17" s="55"/>
-      <c r="D17" s="55"/>
+      <c r="F16" s="61"/>
+      <c r="G16" s="62"/>
+    </row>
+    <row r="17" spans="1:7" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="56"/>
+      <c r="B17" s="56"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="56"/>
       <c r="E17" s="6"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="41"/>
-    </row>
-    <row r="18" spans="1:7" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="55"/>
-      <c r="B18" s="55"/>
-      <c r="C18" s="55"/>
-      <c r="D18" s="55"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="43"/>
+    </row>
+    <row r="18" spans="1:7" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="56"/>
+      <c r="B18" s="56"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="56"/>
       <c r="E18" s="6"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="43"/>
-    </row>
-    <row r="19" spans="1:7" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="55"/>
-      <c r="B19" s="55"/>
-      <c r="C19" s="55"/>
-      <c r="D19" s="55"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="45"/>
+    </row>
+    <row r="19" spans="1:7" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="56"/>
+      <c r="B19" s="56"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="56"/>
       <c r="E19" s="6"/>
-      <c r="F19" s="42"/>
-      <c r="G19" s="43"/>
-    </row>
-    <row r="20" spans="1:7" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F19" s="44"/>
+      <c r="G19" s="45"/>
+    </row>
+    <row r="20" spans="1:7" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
-      <c r="D20" s="25"/>
+      <c r="D20" s="24"/>
       <c r="E20" s="6"/>
-      <c r="F20" s="42"/>
-      <c r="G20" s="43"/>
-    </row>
-    <row r="21" spans="1:7" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="26" t="s">
+      <c r="F20" s="44"/>
+      <c r="G20" s="45"/>
+    </row>
+    <row r="21" spans="1:7" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="25" t="s">
         <v>11</v>
       </c>
       <c r="E21" s="6"/>
-      <c r="F21" s="44"/>
-      <c r="G21" s="45"/>
-    </row>
-    <row r="22" spans="1:7" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:7" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F21" s="46"/>
+      <c r="G21" s="47"/>
+    </row>
+    <row r="22" spans="1:7" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:7" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
-      <c r="F23" s="27" t="s">
+      <c r="F23" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="G23" s="50"/>
-    </row>
-    <row r="24" spans="1:7" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="26" t="s">
+      <c r="G23" s="48"/>
+    </row>
+    <row r="24" spans="1:7" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="F24" s="28" t="s">
+      <c r="F24" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="G24" s="51"/>
-    </row>
-    <row r="25" spans="1:7" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G25" s="29"/>
+      <c r="G24" s="49"/>
+    </row>
+    <row r="25" spans="1:7" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G25" s="28"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
+      <c r="B27" s="57"/>
+      <c r="C27" s="57"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="57"/>
       <c r="F27" s="2"/>
     </row>
     <row r="28" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1360,8 +1359,8 @@
         <v>1</v>
       </c>
       <c r="B29" s="5"/>
-      <c r="C29" s="56"/>
-      <c r="D29" s="57"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="37"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="7"/>
@@ -1374,19 +1373,19 @@
         <v>3</v>
       </c>
       <c r="B31" s="11"/>
-      <c r="C31" s="58"/>
-      <c r="D31" s="59"/>
-    </row>
-    <row r="32" spans="1:7" s="30" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C31" s="30"/>
+      <c r="D31" s="31"/>
+    </row>
+    <row r="32" spans="1:7" s="29" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="12" t="s">
         <v>6</v>
       </c>
       <c r="B32" s="13"/>
-      <c r="C32" s="60"/>
-      <c r="D32" s="61"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="33"/>
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="1:7" s="30" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" s="29" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="14"/>
       <c r="B33" s="14"/>
       <c r="C33" s="14"/>
@@ -1394,188 +1393,171 @@
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
     </row>
-    <row r="34" spans="1:7" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="15" t="s">
+    <row r="34" spans="1:7" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B34" s="5"/>
-      <c r="C34" s="62"/>
-      <c r="D34" s="63"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="35"/>
       <c r="E34" s="6"/>
-      <c r="F34" s="54" t="s">
+      <c r="F34" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="G34" s="50"/>
-    </row>
-    <row r="35" spans="1:7" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G34" s="48"/>
+    </row>
+    <row r="35" spans="1:7" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
-      <c r="B35" s="16"/>
-      <c r="C35" s="16"/>
-      <c r="D35" s="17"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="16"/>
       <c r="E35" s="6"/>
-      <c r="F35" s="33"/>
-      <c r="G35" s="35"/>
-    </row>
-    <row r="36" spans="1:7" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F35" s="51"/>
+      <c r="G35" s="52"/>
+    </row>
+    <row r="36" spans="1:7" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B36" s="11"/>
-      <c r="C36" s="58"/>
-      <c r="D36" s="59"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="31"/>
       <c r="E36" s="6"/>
-      <c r="F36" s="32" t="s">
+      <c r="F36" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="G36" s="52" t="s">
+      <c r="G36" s="54" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:7" s="30" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" s="29" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="12" t="s">
         <v>6</v>
       </c>
       <c r="B37" s="13"/>
-      <c r="C37" s="60"/>
-      <c r="D37" s="61"/>
+      <c r="C37" s="32"/>
+      <c r="D37" s="33"/>
       <c r="E37" s="6"/>
-      <c r="F37" s="33"/>
-      <c r="G37" s="53"/>
-    </row>
-    <row r="38" spans="1:7" s="30" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F37" s="51"/>
+      <c r="G37" s="55"/>
+    </row>
+    <row r="38" spans="1:7" s="29" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="14"/>
       <c r="B38" s="14"/>
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
       <c r="E38" s="6"/>
-      <c r="F38" s="32" t="s">
+      <c r="F38" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="G38" s="34"/>
-    </row>
-    <row r="39" spans="1:7" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="21" t="s">
+      <c r="G38" s="58"/>
+    </row>
+    <row r="39" spans="1:7" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B39" s="22"/>
-      <c r="C39" s="46"/>
-      <c r="D39" s="47"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="38"/>
+      <c r="D39" s="39"/>
       <c r="E39" s="6"/>
-      <c r="F39" s="33"/>
-      <c r="G39" s="35"/>
-    </row>
-    <row r="40" spans="1:7" s="30" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="23"/>
-      <c r="B40" s="24"/>
-      <c r="C40" s="48"/>
-      <c r="D40" s="49"/>
+      <c r="F39" s="51"/>
+      <c r="G39" s="52"/>
+    </row>
+    <row r="40" spans="1:7" s="29" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="22"/>
+      <c r="B40" s="23"/>
+      <c r="C40" s="40"/>
+      <c r="D40" s="41"/>
       <c r="E40" s="6"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="19"/>
-    </row>
-    <row r="41" spans="1:7" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F40" s="17"/>
+      <c r="G40" s="18"/>
+    </row>
+    <row r="41" spans="1:7" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E41" s="6"/>
-      <c r="F41" s="36" t="s">
+      <c r="F41" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="G41" s="37"/>
-    </row>
-    <row r="42" spans="1:7" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="55" t="s">
+      <c r="G41" s="60"/>
+    </row>
+    <row r="42" spans="1:7" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="B42" s="55"/>
-      <c r="C42" s="55"/>
-      <c r="D42" s="55"/>
+      <c r="B42" s="56"/>
+      <c r="C42" s="56"/>
+      <c r="D42" s="56"/>
       <c r="E42" s="6"/>
-      <c r="F42" s="38"/>
-      <c r="G42" s="39"/>
-    </row>
-    <row r="43" spans="1:7" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="55"/>
-      <c r="B43" s="55"/>
-      <c r="C43" s="55"/>
-      <c r="D43" s="55"/>
+      <c r="F42" s="61"/>
+      <c r="G42" s="62"/>
+    </row>
+    <row r="43" spans="1:7" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="56"/>
+      <c r="B43" s="56"/>
+      <c r="C43" s="56"/>
+      <c r="D43" s="56"/>
       <c r="E43" s="6"/>
-      <c r="F43" s="40"/>
-      <c r="G43" s="41"/>
-    </row>
-    <row r="44" spans="1:7" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="55"/>
-      <c r="B44" s="55"/>
-      <c r="C44" s="55"/>
-      <c r="D44" s="55"/>
+      <c r="F43" s="42"/>
+      <c r="G43" s="43"/>
+    </row>
+    <row r="44" spans="1:7" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="56"/>
+      <c r="B44" s="56"/>
+      <c r="C44" s="56"/>
+      <c r="D44" s="56"/>
       <c r="E44" s="6"/>
-      <c r="F44" s="42"/>
-      <c r="G44" s="43"/>
-    </row>
-    <row r="45" spans="1:7" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="55"/>
-      <c r="B45" s="55"/>
-      <c r="C45" s="55"/>
-      <c r="D45" s="55"/>
+      <c r="F44" s="44"/>
+      <c r="G44" s="45"/>
+    </row>
+    <row r="45" spans="1:7" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="56"/>
+      <c r="B45" s="56"/>
+      <c r="C45" s="56"/>
+      <c r="D45" s="56"/>
       <c r="E45" s="6"/>
-      <c r="F45" s="42"/>
-      <c r="G45" s="43"/>
-    </row>
-    <row r="46" spans="1:7" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F45" s="44"/>
+      <c r="G45" s="45"/>
+    </row>
+    <row r="46" spans="1:7" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
-      <c r="D46" s="25"/>
+      <c r="D46" s="24"/>
       <c r="E46" s="6"/>
-      <c r="F46" s="42"/>
-      <c r="G46" s="43"/>
-    </row>
-    <row r="47" spans="1:7" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="26" t="s">
+      <c r="F46" s="44"/>
+      <c r="G46" s="45"/>
+    </row>
+    <row r="47" spans="1:7" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="25" t="s">
         <v>11</v>
       </c>
       <c r="E47" s="6"/>
-      <c r="F47" s="44"/>
-      <c r="G47" s="45"/>
-    </row>
-    <row r="48" spans="1:7" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" spans="1:7" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F47" s="46"/>
+      <c r="G47" s="47"/>
+    </row>
+    <row r="48" spans="1:7" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" spans="1:7" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="8"/>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
-      <c r="F49" s="27" t="s">
+      <c r="F49" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="G49" s="50"/>
-    </row>
-    <row r="50" spans="1:7" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="26" t="s">
+      <c r="G49" s="48"/>
+    </row>
+    <row r="50" spans="1:7" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="F50" s="28" t="s">
+      <c r="F50" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="G50" s="51"/>
-    </row>
-    <row r="51" spans="1:7" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G51" s="29"/>
+      <c r="G50" s="49"/>
+    </row>
+    <row r="51" spans="1:7" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G51" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="C5:D6"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C31:D32"/>
-    <mergeCell ref="C39:D40"/>
-    <mergeCell ref="C13:D14"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="F43:G47"/>
-    <mergeCell ref="G49:G50"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="C36:D37"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="G36:G37"/>
-    <mergeCell ref="A16:D19"/>
-    <mergeCell ref="A42:D45"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A27:E27"/>
     <mergeCell ref="F38:F39"/>
@@ -1591,6 +1573,23 @@
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="F10:F11"/>
+    <mergeCell ref="C39:D40"/>
+    <mergeCell ref="C13:D14"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="F43:G47"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="C36:D37"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="G36:G37"/>
+    <mergeCell ref="A16:D19"/>
+    <mergeCell ref="A42:D45"/>
+    <mergeCell ref="C5:D6"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C31:D32"/>
   </mergeCells>
   <pageMargins left="0.26041666666666669" right="0.25" top="0.21875" bottom="0.17241379310344829" header="0.3" footer="7.1839080459770114E-3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>